<commit_message>
Add SearchMenu and fixed InlineMenu
</commit_message>
<xml_diff>
--- a/TelegramBot/base.xlsx
+++ b/TelegramBot/base.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>https://upload.wikimedia.org/wikipedia/ru/thumb/e/e7/Jurassic_Park_poster.jpg/800px-Jurassic_Park_poster.jpg</t>
   </si>
@@ -93,9 +93,6 @@
     <t>https://avatars.mds.yandex.net/get-kinopoisk-image/1599028/0b76b2a2-d1c7-4f04-a284-80ff7bb709a4/300x450</t>
   </si>
   <si>
-    <t>Властелин колец: Возвращение короля</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 фэнтези, приключения, драма, боевик</t>
   </si>
@@ -103,9 +100,6 @@
     <t>Повелитель сил тьмы Саурон направляет свою бесчисленную армию под стены Минас-Тирита, крепости Последней Надежды. Он предвкушает близкую победу, но именно это мешает ему заметить две крохотные фигурки — хоббитов, приближающихся к Роковой Горе, где им предстоит уничтожить Кольцо Всевластья.</t>
   </si>
   <si>
-    <t>https://avatars.mds.yandex.net/get-kinopoisk-image/4303601/e410c71f-baa1-4fe5-bb29-aedb4662f49b/300x450</t>
-  </si>
-  <si>
     <t xml:space="preserve">Интерстеллар </t>
   </si>
   <si>
@@ -117,9 +111,6 @@
   </si>
   <si>
     <t>https://avatars.mds.yandex.net/get-kinopoisk-image/1600647/430042eb-ee69-4818-aed0-a312400a26bf/300x450</t>
-  </si>
-  <si>
-    <t>Властелин колец: Братство Кольца</t>
   </si>
   <si>
     <t>Сказания о Средиземье — это хроника Великой войны за Кольцо, длившейся не одну тысячу лет. Тот, кто владел Кольцом, получал неограниченную власть, но был обязан служить злу.
@@ -293,6 +284,18 @@
   </si>
   <si>
     <t>https://avatars.mds.yandex.net/get-kinopoisk-image/1599028/4b27e219-a8a5-4d85-9874-57d6016e0837/300x450</t>
+  </si>
+  <si>
+    <t>фэнтези, приключения, драма, боевик</t>
+  </si>
+  <si>
+    <t>Властелин колец  Братство Кольца</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Властелин колец  </t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-kinopoisk-image/4303601/e410c71f-baa1-4fe5-bb29-aedb4662f49b/300x450</t>
   </si>
 </sst>
 </file>
@@ -696,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -791,15 +794,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>8.6999999999999993</v>
@@ -808,18 +811,18 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="D6">
         <v>8.6</v>
@@ -828,18 +831,18 @@
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>8.57</v>
@@ -848,18 +851,18 @@
         <v>1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D8">
         <v>8.7899999999999991</v>
@@ -868,18 +871,18 @@
         <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D9">
         <v>8.8000000000000007</v>
@@ -888,18 +891,18 @@
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10">
         <v>8.69</v>
@@ -908,18 +911,18 @@
         <v>1</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11">
         <v>8.6</v>
@@ -928,18 +931,18 @@
         <v>1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>8.5</v>
@@ -948,18 +951,18 @@
         <v>1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <v>8.4</v>
@@ -968,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -977,17 +980,16 @@
     <hyperlink ref="F2" r:id="rId2"/>
     <hyperlink ref="F4" r:id="rId3"/>
     <hyperlink ref="F3" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="F11" r:id="rId9"/>
-    <hyperlink ref="F12" r:id="rId10"/>
-    <hyperlink ref="F13" r:id="rId11"/>
-    <hyperlink ref="F7" r:id="rId12"/>
-    <hyperlink ref="F8" r:id="rId13"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="F11" r:id="rId8"/>
+    <hyperlink ref="F12" r:id="rId9"/>
+    <hyperlink ref="F13" r:id="rId10"/>
+    <hyperlink ref="F7" r:id="rId11"/>
+    <hyperlink ref="F8" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>